<commit_message>
add 2 immuno networks
</commit_message>
<xml_diff>
--- a/Assignments/Assignment4/HW4_results.xlsx
+++ b/Assignments/Assignment4/HW4_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dmohler\NeuralNets\gitCode\Assignments\Assignment4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DRM_NeuralNets\Neural_Networks\Assignments\Assignment4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Network </t>
   </si>
@@ -71,14 +71,23 @@
     <t>Cross Validation Accuracy (%)</t>
   </si>
   <si>
-    <t>6,12,6</t>
+    <t>Momentum</t>
+  </si>
+  <si>
+    <t>18,24,18</t>
+  </si>
+  <si>
+    <t>100,75,50,25,10,5,2</t>
+  </si>
+  <si>
+    <t>Adagrad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +99,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,9 +132,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,13 +426,13 @@
   <dimension ref="C2:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -416,90 +441,144 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>36</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>5000</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>0.25</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>77.77</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>66.67</v>
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4">
-        <v>5000</v>
+      <c r="I4" s="1">
+        <v>83.33</v>
+      </c>
+      <c r="J4" s="1">
+        <v>72.22</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D5" s="3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3">
+        <v>83.33</v>
+      </c>
+      <c r="J5" s="3">
+        <v>83.33</v>
+      </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add networks and results
</commit_message>
<xml_diff>
--- a/Assignments/Assignment4/HW4_results.xlsx
+++ b/Assignments/Assignment4/HW4_results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DRM_NeuralNets\Neural_Networks\Assignments\Assignment4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Student Files\NeuralNetworks\Neural_Networks\Assignments\Assignment4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F083DBD3-3935-4569-9465-19BFFDFA796F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8088" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t xml:space="preserve">Network </t>
   </si>
@@ -62,9 +63,6 @@
     <t>Learning Rate</t>
   </si>
   <si>
-    <t>Gradient Descent</t>
-  </si>
-  <si>
     <t>Validation Accuracy (%)</t>
   </si>
   <si>
@@ -81,13 +79,46 @@
   </si>
   <si>
     <t>AdaDelta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I1 </t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>CROSS</t>
+  </si>
+  <si>
+    <t>SAME</t>
+  </si>
+  <si>
+    <t>avg over 10 trials</t>
+  </si>
+  <si>
+    <t>Momentum</t>
+  </si>
+  <si>
+    <t>10,15,20,15,10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +138,19 @@
       <b/>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -141,6 +185,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -422,51 +472,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -480,19 +535,19 @@
         <v>5000</v>
       </c>
       <c r="G3" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1">
-        <v>77.77</v>
-      </c>
-      <c r="J3" s="1">
-        <v>66.67</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+        <v>78.89</v>
+      </c>
+      <c r="J3" s="5">
+        <v>68.33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
@@ -500,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1">
         <v>10000</v>
@@ -509,70 +564,100 @@
         <v>0.1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="1">
-        <v>83.33</v>
-      </c>
-      <c r="J4" s="1">
-        <v>72.22</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3">
+        <v>79.44</v>
+      </c>
+      <c r="J4" s="5">
+        <v>68.33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="3">
-        <v>83.33</v>
+      <c r="I5" s="5">
+        <v>71.11</v>
       </c>
       <c r="J5" s="3">
-        <v>83.33</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+        <v>74.989999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1">
+        <v>83.33</v>
+      </c>
+      <c r="J6" s="1">
+        <v>54.45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1">
+        <v>83.33</v>
+      </c>
+      <c r="J7" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -580,6 +665,446 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>83.33</v>
+      </c>
+      <c r="D11">
+        <v>72.22</v>
+      </c>
+      <c r="E11">
+        <v>66.67</v>
+      </c>
+      <c r="F11">
+        <v>83.33</v>
+      </c>
+      <c r="G11">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>77.78</v>
+      </c>
+      <c r="D12">
+        <v>77.78</v>
+      </c>
+      <c r="E12">
+        <v>72.22</v>
+      </c>
+      <c r="F12">
+        <v>83.33</v>
+      </c>
+      <c r="G12">
+        <v>77.77</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>77.78</v>
+      </c>
+      <c r="D13">
+        <v>77.78</v>
+      </c>
+      <c r="E13">
+        <v>66.67</v>
+      </c>
+      <c r="F13">
+        <v>83.33</v>
+      </c>
+      <c r="G13">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>77.78</v>
+      </c>
+      <c r="D14">
+        <v>77.78</v>
+      </c>
+      <c r="E14">
+        <v>77.78</v>
+      </c>
+      <c r="F14">
+        <v>83.33</v>
+      </c>
+      <c r="G14">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>77.78</v>
+      </c>
+      <c r="D15">
+        <v>83.33</v>
+      </c>
+      <c r="E15">
+        <v>77.78</v>
+      </c>
+      <c r="F15">
+        <v>77.77</v>
+      </c>
+      <c r="G15">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>77.78</v>
+      </c>
+      <c r="D16">
+        <v>77.78</v>
+      </c>
+      <c r="E16">
+        <v>66.67</v>
+      </c>
+      <c r="F16">
+        <v>88.89</v>
+      </c>
+      <c r="G16">
+        <v>88.89</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>77.78</v>
+      </c>
+      <c r="D17">
+        <v>83.33</v>
+      </c>
+      <c r="E17">
+        <v>72.22</v>
+      </c>
+      <c r="F17">
+        <v>83.33</v>
+      </c>
+      <c r="G17">
+        <v>88.89</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>77.78</v>
+      </c>
+      <c r="D18">
+        <v>83.33</v>
+      </c>
+      <c r="E18">
+        <v>66.67</v>
+      </c>
+      <c r="F18">
+        <v>83.33</v>
+      </c>
+      <c r="G18">
+        <v>77.78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>77.78</v>
+      </c>
+      <c r="D19">
+        <v>77.78</v>
+      </c>
+      <c r="E19">
+        <v>72.22</v>
+      </c>
+      <c r="F19">
+        <v>83.33</v>
+      </c>
+      <c r="G19">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>83.33</v>
+      </c>
+      <c r="D20">
+        <v>83.33</v>
+      </c>
+      <c r="E20">
+        <v>72.22</v>
+      </c>
+      <c r="F20">
+        <v>83.33</v>
+      </c>
+      <c r="G20">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f>AVERAGE(C11:C20)</f>
+        <v>78.89</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:H21" si="0">AVERAGE(D11:D20)</f>
+        <v>79.444000000000003</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>71.111999999999995</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>83.330000000000013</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>83.331000000000003</v>
+      </c>
+      <c r="H21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>66.67</v>
+      </c>
+      <c r="D26">
+        <v>66.67</v>
+      </c>
+      <c r="E26">
+        <v>83.33</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
+      </c>
+      <c r="G26">
+        <v>55.56</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>66.67</v>
+      </c>
+      <c r="D27">
+        <v>66.67</v>
+      </c>
+      <c r="E27">
+        <v>77.77</v>
+      </c>
+      <c r="F27">
+        <v>50</v>
+      </c>
+      <c r="G27">
+        <v>72.22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>66.67</v>
+      </c>
+      <c r="D28">
+        <v>61.11</v>
+      </c>
+      <c r="E28">
+        <v>83.33</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>66.67</v>
+      </c>
+      <c r="D29">
+        <v>72.22</v>
+      </c>
+      <c r="E29">
+        <v>72.22</v>
+      </c>
+      <c r="F29">
+        <v>66.67</v>
+      </c>
+      <c r="G29">
+        <v>77.77</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>72.22</v>
+      </c>
+      <c r="D30">
+        <v>72.22</v>
+      </c>
+      <c r="E30">
+        <v>66.67</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>55.56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>72.22</v>
+      </c>
+      <c r="D31">
+        <v>66.67</v>
+      </c>
+      <c r="E31">
+        <v>66.67</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>72.22</v>
+      </c>
+      <c r="D32">
+        <v>72.22</v>
+      </c>
+      <c r="E32">
+        <v>72.22</v>
+      </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32">
+        <v>83.33</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>72.22</v>
+      </c>
+      <c r="D33">
+        <v>66.67</v>
+      </c>
+      <c r="E33">
+        <v>77.77</v>
+      </c>
+      <c r="F33">
+        <v>61.11</v>
+      </c>
+      <c r="G33">
+        <v>77.78</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>66.67</v>
+      </c>
+      <c r="D34">
+        <v>72.22</v>
+      </c>
+      <c r="E34">
+        <v>72.22</v>
+      </c>
+      <c r="F34">
+        <v>66.67</v>
+      </c>
+      <c r="G34">
+        <v>72.22</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>61.11</v>
+      </c>
+      <c r="D35">
+        <v>66.67</v>
+      </c>
+      <c r="E35">
+        <v>77.77</v>
+      </c>
+      <c r="F35">
+        <v>50</v>
+      </c>
+      <c r="G35">
+        <v>55.56</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f>AVERAGE(C26:C35)</f>
+        <v>68.334000000000003</v>
+      </c>
+      <c r="D36">
+        <f>AVERAGE(D26:D35)</f>
+        <v>68.333999999999989</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ref="E36:H36" si="1">AVERAGE(E26:E35)</f>
+        <v>74.997</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>54.445000000000007</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H36" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>